<commit_message>
Some cleanup of the documentation file, plus a change to FERT (per Clem)
</commit_message>
<xml_diff>
--- a/src/class_FERT/results_template.xlsx
+++ b/src/class_FERT/results_template.xlsx
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,14 +404,12 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>G1&lt;&gt;F1</formula>
     </cfRule>
@@ -425,7 +419,7 @@
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576 I1:I1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
@@ -453,31 +447,14 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="I1 G1:G1048576 I3:I1048576">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>G1&lt;&gt;F1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>I2&lt;&gt;H2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>$C1=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="expression" priority="1" stopIfTrue="1">
-      <formula>F1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">

</xml_diff>